<commit_message>
Updated WASM results and extended Emscripten build instructions in README
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -484,13 +484,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.4867300000000001</c:v>
+                  <c:v>3.1086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.2935600000000003</c:v>
+                  <c:v>4.9429629999999989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3722299999999983</c:v>
+                  <c:v>7.6752519999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8.192029999999999</c:v>
@@ -557,11 +557,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="246120448"/>
-        <c:axId val="246122368"/>
+        <c:axId val="246317056"/>
+        <c:axId val="246318976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="246120448"/>
+        <c:axId val="246317056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,7 +596,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246122368"/>
+        <c:crossAx val="246318976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -604,7 +604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246122368"/>
+        <c:axId val="246318976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -660,7 +660,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="246120448"/>
+        <c:crossAx val="246317056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1038,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1184,13 +1184,13 @@
         <v>0.67352599999999996</v>
       </c>
       <c r="H6">
-        <v>3.4516</v>
+        <v>3.0752999999999999</v>
       </c>
       <c r="I6">
-        <v>5.2531999999999996</v>
+        <v>5.0811299999999999</v>
       </c>
       <c r="J6">
-        <v>8.5040999999999993</v>
+        <v>7.633</v>
       </c>
       <c r="K6">
         <v>8.0498999999999992</v>
@@ -1219,13 +1219,13 @@
         <v>0.67976899999999996</v>
       </c>
       <c r="H7">
-        <v>3.3321999999999998</v>
+        <v>3.0070000000000001</v>
       </c>
       <c r="I7">
-        <v>5.0914000000000001</v>
+        <v>4.8851000000000004</v>
       </c>
       <c r="J7">
-        <v>8.2010000000000005</v>
+        <v>8.1645000000000003</v>
       </c>
       <c r="K7">
         <v>8.0622000000000007</v>
@@ -1254,13 +1254,13 @@
         <v>0.65806900000000002</v>
       </c>
       <c r="H8">
-        <v>3.37</v>
+        <v>3.3279999999999998</v>
       </c>
       <c r="I8">
-        <v>5.2553999999999998</v>
+        <v>4.7542</v>
       </c>
       <c r="J8">
-        <v>8.3825000000000003</v>
+        <v>7.5202</v>
       </c>
       <c r="K8">
         <v>8.3071999999999999</v>
@@ -1289,13 +1289,13 @@
         <v>0.65804200000000002</v>
       </c>
       <c r="H9">
-        <v>3.4241999999999999</v>
+        <v>2.9969999999999999</v>
       </c>
       <c r="I9">
-        <v>5.1017999999999999</v>
+        <v>5.0053999999999998</v>
       </c>
       <c r="J9">
-        <v>8.3991000000000007</v>
+        <v>7.5201200000000004</v>
       </c>
       <c r="K9">
         <v>8.0754000000000001</v>
@@ -1324,13 +1324,13 @@
         <v>0.66747999999999996</v>
       </c>
       <c r="H10">
-        <v>3.3378999999999999</v>
+        <v>3.0217000000000001</v>
       </c>
       <c r="I10">
-        <v>5.5746000000000002</v>
+        <v>4.9242999999999997</v>
       </c>
       <c r="J10">
-        <v>8.3170000000000002</v>
+        <v>7.8101000000000003</v>
       </c>
       <c r="K10">
         <v>8.3209999999999997</v>
@@ -1359,13 +1359,13 @@
         <v>0.65725900000000004</v>
       </c>
       <c r="H11">
-        <v>3.7984</v>
+        <v>3.0537999999999998</v>
       </c>
       <c r="I11">
-        <v>5.282</v>
+        <v>4.8785999999999996</v>
       </c>
       <c r="J11">
-        <v>8.4075000000000006</v>
+        <v>7.5704000000000002</v>
       </c>
       <c r="K11">
         <v>8.0713000000000008</v>
@@ -1394,13 +1394,13 @@
         <v>0.68001599999999995</v>
       </c>
       <c r="H12">
-        <v>3.3508</v>
+        <v>2.9979</v>
       </c>
       <c r="I12">
-        <v>5.3468999999999998</v>
+        <v>4.9705000000000004</v>
       </c>
       <c r="J12">
-        <v>8.4146999999999998</v>
+        <v>7.5528000000000004</v>
       </c>
       <c r="K12">
         <v>8.3594000000000008</v>
@@ -1429,13 +1429,13 @@
         <v>0.65775799999999995</v>
       </c>
       <c r="H13">
-        <v>3.3136999999999999</v>
+        <v>3.2791000000000001</v>
       </c>
       <c r="I13">
-        <v>5.3810000000000002</v>
+        <v>5.0410000000000004</v>
       </c>
       <c r="J13">
-        <v>8.1347000000000005</v>
+        <v>7.6109999999999998</v>
       </c>
       <c r="K13">
         <v>8.2269000000000005</v>
@@ -1464,13 +1464,13 @@
         <v>0.66896</v>
       </c>
       <c r="H14">
-        <v>3.8277999999999999</v>
+        <v>3.2896000000000001</v>
       </c>
       <c r="I14">
-        <v>5.2995000000000001</v>
+        <v>5.0373999999999999</v>
       </c>
       <c r="J14">
-        <v>8.6506000000000007</v>
+        <v>7.6349999999999998</v>
       </c>
       <c r="K14">
         <v>8.1708999999999996</v>
@@ -1499,13 +1499,13 @@
         <v>0.65363700000000002</v>
       </c>
       <c r="H15" s="1">
-        <v>3.6606999999999998</v>
+        <v>3.0366</v>
       </c>
       <c r="I15" s="1">
-        <v>5.3498000000000001</v>
+        <v>4.8520000000000003</v>
       </c>
       <c r="J15" s="1">
-        <v>8.3110999999999997</v>
+        <v>7.7354000000000003</v>
       </c>
       <c r="K15" s="1">
         <v>8.2760999999999996</v>
@@ -1544,15 +1544,15 @@
       </c>
       <c r="H16" s="2">
         <f t="shared" ref="H16:K16" si="1">AVERAGE(H6:H15)</f>
-        <v>3.4867300000000001</v>
+        <v>3.1086</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="1"/>
-        <v>5.2935600000000003</v>
+        <v>4.9429629999999989</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="1"/>
-        <v>8.3722299999999983</v>
+        <v>7.6752519999999986</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="1"/>
@@ -1593,15 +1593,15 @@
       <c r="H17" s="5"/>
       <c r="I17" s="6">
         <f>$H16/I16</f>
-        <v>0.65867393587680123</v>
+        <v>0.62889404593965215</v>
       </c>
       <c r="J17" s="6">
         <f t="shared" ref="J17:K17" si="4">$H16/J16</f>
-        <v>0.41646371396867987</v>
+        <v>0.40501601771511875</v>
       </c>
       <c r="K17" s="6">
         <f t="shared" si="4"/>
-        <v>0.42562466201906007</v>
+        <v>0.37946638379009845</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="6"/>
@@ -1639,7 +1639,7 @@
       </c>
       <c r="C22" s="2">
         <f>$H$16</f>
-        <v>3.4867300000000001</v>
+        <v>3.1086</v>
       </c>
       <c r="D22" s="2">
         <f>$M$16</f>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="C23" s="2">
         <f>$I$16</f>
-        <v>5.2935600000000003</v>
+        <v>4.9429629999999989</v>
       </c>
       <c r="D23" s="2"/>
     </row>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="C24" s="2">
         <f>$J$16</f>
-        <v>8.3722299999999983</v>
+        <v>7.6752519999999986</v>
       </c>
       <c r="D24" s="2"/>
     </row>

</xml_diff>

<commit_message>
Pre-allocate left/right arrays in JS
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -165,13 +165,13 @@
     <t>FireFox</t>
   </si>
   <si>
-    <t>Kotlin</t>
-  </si>
-  <si>
     <t>JVM</t>
   </si>
   <si>
     <t>Native</t>
+  </si>
+  <si>
+    <t>Kotlin (Ubuntu 18.04)</t>
   </si>
 </sst>
 </file>
@@ -273,6 +273,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -283,9 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,7 +616,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>4.6917</c:v>
+                  <c:v>2.6150000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -653,7 +653,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2.2000000000000002</c:v>
+                  <c:v>1.87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -677,11 +677,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193198336"/>
-        <c:axId val="193548672"/>
+        <c:axId val="237374848"/>
+        <c:axId val="237397504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193198336"/>
+        <c:axId val="237374848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,7 +716,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193548672"/>
+        <c:crossAx val="237397504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -724,7 +724,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193548672"/>
+        <c:axId val="237397504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9"/>
@@ -780,7 +780,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="193198336"/>
+        <c:crossAx val="237374848"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1162,8 +1162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1189,103 +1189,103 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="H2" s="15" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="H2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
       <c r="L2" s="10"/>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="15" t="s">
+      <c r="R2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="H3" s="16" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="H3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
       <c r="Q3" s="11"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="H4" s="17" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="H4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
       <c r="L4" s="12"/>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="12"/>
-      <c r="R4" s="17" t="s">
+      <c r="R4" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
     </row>
     <row r="5" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="19"/>
       <c r="I5" s="3">
         <v>2</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="14"/>
-      <c r="M5" s="18"/>
+      <c r="M5" s="19"/>
       <c r="N5" s="3">
         <v>2</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="14"/>
-      <c r="R5" s="18"/>
+      <c r="R5" s="19"/>
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
@@ -1372,7 +1372,7 @@
         <v>6.8239999999999998</v>
       </c>
       <c r="R6">
-        <v>4.6207000000000003</v>
+        <v>2.6680000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -1419,7 +1419,7 @@
         <v>6.5890000000000004</v>
       </c>
       <c r="R7">
-        <v>4.7789000000000001</v>
+        <v>2.6509999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>6.6660000000000004</v>
       </c>
       <c r="R8">
-        <v>4.6974999999999998</v>
+        <v>2.6230000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -1513,7 +1513,7 @@
         <v>6.798</v>
       </c>
       <c r="R9">
-        <v>4.6584000000000003</v>
+        <v>2.61</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -1560,7 +1560,7 @@
         <v>6.6079999999999997</v>
       </c>
       <c r="R10">
-        <v>4.6256000000000004</v>
+        <v>2.6019999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -1607,7 +1607,7 @@
         <v>6.72</v>
       </c>
       <c r="R11">
-        <v>4.7275</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -1654,7 +1654,7 @@
         <v>6.5149999999999997</v>
       </c>
       <c r="R12">
-        <v>4.8407</v>
+        <v>2.6339999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -1701,7 +1701,7 @@
         <v>6.6769999999999996</v>
       </c>
       <c r="R13">
-        <v>4.6513999999999998</v>
+        <v>2.54</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -1748,7 +1748,7 @@
         <v>6.6120000000000001</v>
       </c>
       <c r="R14">
-        <v>4.6624999999999996</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
       </c>
       <c r="Q15" s="9"/>
       <c r="R15" s="1">
-        <v>4.6538000000000004</v>
+        <v>2.6019999999999999</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
@@ -1864,7 +1864,7 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2">
         <f t="shared" ref="R16" si="3">AVERAGE(R6:R15)</f>
-        <v>4.6917</v>
+        <v>2.6150000000000002</v>
       </c>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
@@ -1938,15 +1938,15 @@
       <c r="F18" s="6"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="F20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="F20" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
@@ -1962,10 +1962,10 @@
         <v>14</v>
       </c>
       <c r="F21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
@@ -1986,13 +1986,13 @@
       </c>
       <c r="E22" s="2">
         <f>$R$16</f>
-        <v>4.6917</v>
+        <v>2.6150000000000002</v>
       </c>
       <c r="F22">
-        <v>2.2000000000000002</v>
+        <v>1.87</v>
       </c>
       <c r="H22">
-        <v>35</v>
+        <v>9.1999999999999993</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -2051,6 +2051,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="C20:D20"/>
@@ -2067,8 +2069,6 @@
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M4:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="landscape" copies="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Preallocate temporary array (in all languages)
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Built with:</t>
-  </si>
-  <si>
-    <t>JS</t>
   </si>
   <si>
     <r>
@@ -159,19 +156,22 @@
     <t>WebAssembly in FireFox v65 (64-bit)</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>FireFox</t>
-  </si>
-  <si>
-    <t>JVM</t>
-  </si>
-  <si>
     <t>Native</t>
   </si>
   <si>
     <t>Kotlin (Ubuntu 18.04)</t>
+  </si>
+  <si>
+    <t>WASM Chrome</t>
+  </si>
+  <si>
+    <t>WASM FF</t>
+  </si>
+  <si>
+    <t>JS Chrome</t>
+  </si>
+  <si>
+    <t>Kotlin/JVM</t>
   </si>
 </sst>
 </file>
@@ -251,9 +251,6 @@
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -273,12 +270,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -286,6 +277,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -358,7 +358,7 @@
           <c:x val="0.14759313600753102"/>
           <c:y val="9.3272205462669538E-2"/>
           <c:w val="0.7946303960163521"/>
-          <c:h val="0.70767551973233334"/>
+          <c:h val="0.76274574198612"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -434,16 +434,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.79619</c:v>
+                  <c:v>1.5499500000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98401139999999998</c:v>
+                  <c:v>0.79174560000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.61754870000000017</c:v>
+                  <c:v>0.45439160000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.66545160000000003</c:v>
+                  <c:v>0.45939300000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,7 +478,8 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -510,16 +511,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.1086</c:v>
+                  <c:v>2.3837999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9429629999999989</c:v>
+                  <c:v>1.2170000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6752519999999986</c:v>
+                  <c:v>0.71250000000000013</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.192029999999999</c:v>
+                  <c:v>0.73369999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -563,7 +564,8 @@
                 </a:solidFill>
               </a:ln>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -574,16 +576,16 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.3241999999999989</c:v>
+                  <c:v>3.1560999999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2553000000000001</c:v>
+                  <c:v>1.5948</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5561000000000007</c:v>
+                  <c:v>0.95479999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6692000000000009</c:v>
+                  <c:v>0.96449999999999991</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -594,15 +596,7 @@
           <c:idx val="2"/>
           <c:order val="3"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$E$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>JS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>JS Chrome</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575">
@@ -677,11 +671,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="237374848"/>
-        <c:axId val="237397504"/>
+        <c:axId val="233643392"/>
+        <c:axId val="233666048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="237374848"/>
+        <c:axId val="233643392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -716,7 +710,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="237397504"/>
+        <c:crossAx val="233666048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -724,10 +718,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="237397504"/>
+        <c:axId val="233666048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="9"/>
+          <c:max val="3.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -780,7 +774,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="237374848"/>
+        <c:crossAx val="233643392"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -813,8 +807,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17571741286999579"/>
-          <c:y val="0.11208600085530279"/>
+          <c:x val="0.69282616013216702"/>
+          <c:y val="0.12743646216738844"/>
           <c:w val="0.20179136038021825"/>
           <c:h val="0.20598239566089402"/>
         </c:manualLayout>
@@ -838,20 +832,221 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16496097445690047"/>
+          <c:y val="0.12530116139728076"/>
+          <c:w val="0.79597648425047318"/>
+          <c:h val="0.74364858046437876"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>x64</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>WASM Chrome</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>WASM FF</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>JS Chrome</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Kotlin/JVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.5499500000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3837999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1560999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>1.87</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="37035008"/>
+        <c:axId val="37161216"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37035008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37161216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="37161216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="37035008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="F1F6FD"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId1"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>177992</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>171207</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>476164</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>32059</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>396706</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>24243</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>52754</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -870,7 +1065,144 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>414130</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66259</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>212034</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>53008</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4" title="Merge Sort of 10M Floats on Single Thread"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.10569</cdr:x>
+      <cdr:y>0.06119</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.81864</cdr:x>
+      <cdr:y>0.13582</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="559904" y="271672"/>
+          <a:ext cx="3776869" cy="331304"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.23577</cdr:x>
+      <cdr:y>0.03134</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.73608</cdr:x>
+      <cdr:y>0.09851</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1249016" y="139150"/>
+          <a:ext cx="2650435" cy="298174"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Merge Sort of 10M Floats on Single Thread</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02314</cdr:x>
+      <cdr:y>0.31493</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.08693</cdr:x>
+      <cdr:y>0.59702</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 3"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="16200000">
+          <a:off x="-334614" y="1855308"/>
+          <a:ext cx="1252331" cy="337930"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Time, seconds</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1160,66 +1492,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="7.88671875" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="2.44140625" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="10" width="7.5546875" customWidth="1"/>
-    <col min="11" max="11" width="8.21875" customWidth="1"/>
-    <col min="12" max="12" width="3.21875" customWidth="1"/>
-    <col min="13" max="16" width="8.21875" customWidth="1"/>
-    <col min="17" max="17" width="3" customWidth="1"/>
-    <col min="18" max="18" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" customWidth="1"/>
+    <col min="5" max="5" width="4.77734375" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="8" width="7.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.21875" customWidth="1"/>
+    <col min="10" max="10" width="3.21875" customWidth="1"/>
+    <col min="11" max="14" width="8.21875" customWidth="1"/>
+    <col min="15" max="15" width="3" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="H2" s="16" t="s">
+      <c r="F2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="16" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -1227,765 +1555,677 @@
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="H3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>6</v>
       </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
       <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="17" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="17" t="s">
         <v>6</v>
       </c>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
       <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
+      <c r="O3" s="10"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="11"/>
+      <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+    <row r="4" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="H4" s="18" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="F4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="G4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="18" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="L4" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="18" t="s">
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
     </row>
-    <row r="5" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:19" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="16"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="3">
+        <v>2</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="3">
+      <c r="I5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="13"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="3">
         <v>2</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="3">
-        <v>2</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="19"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
       <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>1.7998099999999999</v>
+        <v>1.55823</v>
       </c>
       <c r="B6">
-        <v>0.98813099999999998</v>
+        <v>0.79006699999999996</v>
       </c>
       <c r="C6">
-        <v>0.61828300000000003</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="D6">
-        <v>0.67472100000000002</v>
-      </c>
-      <c r="E6">
-        <v>0.61610399999999998</v>
+        <v>0.45767999999999998</v>
       </c>
       <c r="F6">
-        <v>0.67352599999999996</v>
+        <v>2.371</v>
+      </c>
+      <c r="G6">
+        <v>1.208</v>
       </c>
       <c r="H6">
-        <v>3.0752999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="I6">
-        <v>5.0811299999999999</v>
-      </c>
-      <c r="J6">
-        <v>7.633</v>
+        <v>0.85099999999999998</v>
       </c>
       <c r="K6">
-        <v>8.0498999999999992</v>
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="L6">
+        <v>1.6040000000000001</v>
       </c>
       <c r="M6">
-        <v>3.3029999999999999</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="N6">
-        <v>4.2279999999999998</v>
-      </c>
-      <c r="O6">
-        <v>6.2930000000000001</v>
+        <v>0.96299999999999997</v>
       </c>
       <c r="P6">
-        <v>6.8239999999999998</v>
-      </c>
-      <c r="R6">
         <v>2.6680000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>1.80101</v>
+        <v>1.5446500000000001</v>
       </c>
       <c r="B7">
-        <v>0.99072499999999997</v>
+        <v>0.79332199999999997</v>
       </c>
       <c r="C7">
-        <v>0.62315399999999999</v>
+        <v>0.45422499999999999</v>
       </c>
       <c r="D7">
-        <v>0.66510199999999997</v>
-      </c>
-      <c r="E7">
-        <v>0.61510799999999999</v>
+        <v>0.46072000000000002</v>
       </c>
       <c r="F7">
-        <v>0.67976899999999996</v>
+        <v>2.3620000000000001</v>
+      </c>
+      <c r="G7">
+        <v>1.196</v>
       </c>
       <c r="H7">
-        <v>3.0070000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="I7">
-        <v>4.8851000000000004</v>
-      </c>
-      <c r="J7">
-        <v>8.1645000000000003</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="K7">
-        <v>8.0622000000000007</v>
+        <v>3.1389999999999998</v>
+      </c>
+      <c r="L7">
+        <v>1.585</v>
       </c>
       <c r="M7">
-        <v>3.2429999999999999</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="N7">
-        <v>4.3689999999999998</v>
-      </c>
-      <c r="O7">
-        <v>6.4279999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="P7">
-        <v>6.5890000000000004</v>
-      </c>
-      <c r="R7">
         <v>2.6509999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>1.7961199999999999</v>
+        <v>1.5489900000000001</v>
       </c>
       <c r="B8">
-        <v>0.98679300000000003</v>
+        <v>0.78911200000000004</v>
       </c>
       <c r="C8">
-        <v>0.62917900000000004</v>
+        <v>0.45158599999999999</v>
       </c>
       <c r="D8">
-        <v>0.66562200000000005</v>
-      </c>
-      <c r="E8">
-        <v>0.61862700000000004</v>
+        <v>0.45802999999999999</v>
       </c>
       <c r="F8">
-        <v>0.65806900000000002</v>
+        <v>2.3740000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1.304</v>
       </c>
       <c r="H8">
-        <v>3.3279999999999998</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="I8">
-        <v>4.7542</v>
-      </c>
-      <c r="J8">
-        <v>7.5202</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="K8">
-        <v>8.3071999999999999</v>
+        <v>3.1179999999999999</v>
+      </c>
+      <c r="L8">
+        <v>1.581</v>
       </c>
       <c r="M8">
-        <v>3.3180000000000001</v>
+        <v>0.93600000000000005</v>
       </c>
       <c r="N8">
-        <v>4.0579999999999998</v>
-      </c>
-      <c r="O8">
-        <v>6.6289999999999996</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="P8">
-        <v>6.6660000000000004</v>
-      </c>
-      <c r="R8">
         <v>2.6230000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>1.7966599999999999</v>
+        <v>1.54803</v>
       </c>
       <c r="B9">
-        <v>0.97666299999999995</v>
+        <v>0.79036200000000001</v>
       </c>
       <c r="C9">
-        <v>0.61488399999999999</v>
+        <v>0.46921800000000002</v>
       </c>
       <c r="D9">
-        <v>0.658667</v>
-      </c>
-      <c r="E9">
-        <v>0.62006300000000003</v>
+        <v>0.45971000000000001</v>
       </c>
       <c r="F9">
-        <v>0.65804200000000002</v>
+        <v>2.411</v>
+      </c>
+      <c r="G9">
+        <v>1.2190000000000001</v>
       </c>
       <c r="H9">
-        <v>2.9969999999999999</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="I9">
-        <v>5.0053999999999998</v>
-      </c>
-      <c r="J9">
-        <v>7.5201200000000004</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="K9">
-        <v>8.0754000000000001</v>
+        <v>3.1539999999999999</v>
+      </c>
+      <c r="L9">
+        <v>1.601</v>
       </c>
       <c r="M9">
-        <v>3.3159999999999998</v>
+        <v>0.96399999999999997</v>
       </c>
       <c r="N9">
-        <v>4.3140000000000001</v>
-      </c>
-      <c r="O9">
-        <v>6.4530000000000003</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="P9">
-        <v>6.798</v>
-      </c>
-      <c r="R9">
         <v>2.61</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>1.7904</v>
+        <v>1.54898</v>
       </c>
       <c r="B10">
-        <v>0.98483600000000004</v>
+        <v>0.79872399999999999</v>
       </c>
       <c r="C10">
-        <v>0.62238400000000005</v>
+        <v>0.45121800000000001</v>
       </c>
       <c r="D10">
-        <v>0.66966300000000001</v>
-      </c>
-      <c r="E10">
-        <v>0.62123099999999998</v>
+        <v>0.46045999999999998</v>
       </c>
       <c r="F10">
-        <v>0.66747999999999996</v>
+        <v>2.4169999999999998</v>
+      </c>
+      <c r="G10">
+        <v>1.2050000000000001</v>
       </c>
       <c r="H10">
-        <v>3.0217000000000001</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="I10">
-        <v>4.9242999999999997</v>
-      </c>
-      <c r="J10">
-        <v>7.8101000000000003</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="K10">
-        <v>8.3209999999999997</v>
+        <v>3.121</v>
+      </c>
+      <c r="L10">
+        <v>1.5940000000000001</v>
       </c>
       <c r="M10">
-        <v>3.5219999999999998</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="N10">
-        <v>4.2779999999999996</v>
-      </c>
-      <c r="O10">
-        <v>6.6680000000000001</v>
+        <v>0.96099999999999997</v>
       </c>
       <c r="P10">
-        <v>6.6079999999999997</v>
-      </c>
-      <c r="R10">
         <v>2.6019999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>1.7878099999999999</v>
+        <v>1.55124</v>
       </c>
       <c r="B11">
-        <v>0.98288799999999998</v>
+        <v>0.79605099999999995</v>
       </c>
       <c r="C11">
-        <v>0.62745899999999999</v>
+        <v>0.45399400000000001</v>
       </c>
       <c r="D11">
-        <v>0.67066999999999999</v>
-      </c>
-      <c r="E11">
-        <v>0.621201</v>
+        <v>0.46383999999999997</v>
       </c>
       <c r="F11">
-        <v>0.65725900000000004</v>
+        <v>2.363</v>
+      </c>
+      <c r="G11">
+        <v>1.2190000000000001</v>
       </c>
       <c r="H11">
-        <v>3.0537999999999998</v>
+        <v>0.69899999999999995</v>
       </c>
       <c r="I11">
-        <v>4.8785999999999996</v>
-      </c>
-      <c r="J11">
-        <v>7.5704000000000002</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="K11">
-        <v>8.0713000000000008</v>
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="L11">
+        <v>1.6080000000000001</v>
       </c>
       <c r="M11">
-        <v>3.3159999999999998</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="N11">
-        <v>4.0449999999999999</v>
-      </c>
-      <c r="O11">
-        <v>6.49</v>
+        <v>0.98099999999999998</v>
       </c>
       <c r="P11">
-        <v>6.72</v>
-      </c>
-      <c r="R11">
         <v>2.62</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>1.7903199999999999</v>
+        <v>1.55019</v>
       </c>
       <c r="B12">
-        <v>0.98150599999999999</v>
+        <v>0.78846899999999998</v>
       </c>
       <c r="C12">
-        <v>0.61919999999999997</v>
+        <v>0.45378499999999999</v>
       </c>
       <c r="D12">
-        <v>0.657138</v>
-      </c>
-      <c r="E12">
-        <v>0.62028700000000003</v>
+        <v>0.45833000000000002</v>
       </c>
       <c r="F12">
-        <v>0.68001599999999995</v>
+        <v>2.3809999999999998</v>
+      </c>
+      <c r="G12">
+        <v>1.2030000000000001</v>
       </c>
       <c r="H12">
-        <v>2.9979</v>
+        <v>0.70799999999999996</v>
       </c>
       <c r="I12">
-        <v>4.9705000000000004</v>
-      </c>
-      <c r="J12">
-        <v>7.5528000000000004</v>
+        <v>0.70399999999999996</v>
       </c>
       <c r="K12">
-        <v>8.3594000000000008</v>
+        <v>3.1190000000000002</v>
+      </c>
+      <c r="L12">
+        <v>1.599</v>
       </c>
       <c r="M12">
-        <v>3.2370000000000001</v>
+        <v>0.95499999999999996</v>
       </c>
       <c r="N12">
-        <v>4.3319999999999999</v>
-      </c>
-      <c r="O12">
-        <v>6.7039999999999997</v>
+        <v>0.96199999999999997</v>
       </c>
       <c r="P12">
-        <v>6.5149999999999997</v>
-      </c>
-      <c r="R12">
         <v>2.6339999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>1.78678</v>
+        <v>1.5471900000000001</v>
       </c>
       <c r="B13">
-        <v>0.98906499999999997</v>
+        <v>0.79352199999999995</v>
       </c>
       <c r="C13">
-        <v>0.62900800000000001</v>
+        <v>0.45282099999999997</v>
       </c>
       <c r="D13">
-        <v>0.658748</v>
-      </c>
-      <c r="E13">
-        <v>0.61646699999999999</v>
+        <v>0.45682</v>
       </c>
       <c r="F13">
-        <v>0.65775799999999995</v>
+        <v>2.42</v>
+      </c>
+      <c r="G13">
+        <v>1.21</v>
       </c>
       <c r="H13">
-        <v>3.2791000000000001</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="I13">
-        <v>5.0410000000000004</v>
-      </c>
-      <c r="J13">
-        <v>7.6109999999999998</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="K13">
-        <v>8.2269000000000005</v>
+        <v>3.15</v>
+      </c>
+      <c r="L13">
+        <v>1.593</v>
       </c>
       <c r="M13">
-        <v>3.4350000000000001</v>
+        <v>1.0209999999999999</v>
       </c>
       <c r="N13">
-        <v>4.3259999999999996</v>
-      </c>
-      <c r="O13">
-        <v>6.5620000000000003</v>
+        <v>0.97099999999999997</v>
       </c>
       <c r="P13">
-        <v>6.6769999999999996</v>
-      </c>
-      <c r="R13">
         <v>2.54</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1.7904599999999999</v>
+        <v>1.54572</v>
       </c>
       <c r="B14">
-        <v>0.98244799999999999</v>
+        <v>0.78565600000000002</v>
       </c>
       <c r="C14">
-        <v>0.61516999999999999</v>
+        <v>0.452787</v>
       </c>
       <c r="D14">
-        <v>0.657578</v>
-      </c>
-      <c r="E14">
-        <v>0.60813200000000001</v>
+        <v>0.45961999999999997</v>
       </c>
       <c r="F14">
-        <v>0.66896</v>
+        <v>2.3719999999999999</v>
+      </c>
+      <c r="G14">
+        <v>1.214</v>
       </c>
       <c r="H14">
-        <v>3.2896000000000001</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="I14">
-        <v>5.0373999999999999</v>
-      </c>
-      <c r="J14">
-        <v>7.6349999999999998</v>
+        <v>0.72799999999999998</v>
       </c>
       <c r="K14">
-        <v>8.1708999999999996</v>
+        <v>3.0750000000000002</v>
+      </c>
+      <c r="L14">
+        <v>1.595</v>
       </c>
       <c r="M14">
-        <v>3.3010000000000002</v>
+        <v>0.95199999999999996</v>
       </c>
       <c r="N14">
-        <v>4.2949999999999999</v>
-      </c>
-      <c r="O14">
-        <v>6.6529999999999996</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="P14">
-        <v>6.6120000000000001</v>
-      </c>
-      <c r="R14">
         <v>2.6</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>1.82253</v>
+        <v>1.5562800000000001</v>
       </c>
       <c r="B15" s="1">
-        <v>0.97705900000000001</v>
+        <v>0.79217099999999996</v>
       </c>
       <c r="C15" s="1">
-        <v>0.62984399999999996</v>
+        <v>0.45528200000000002</v>
       </c>
       <c r="D15" s="1">
-        <v>0.71137300000000003</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0.61826700000000001</v>
+        <v>0.45872000000000002</v>
       </c>
       <c r="F15" s="1">
-        <v>0.65363700000000002</v>
+        <v>2.367</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1.1919999999999999</v>
       </c>
       <c r="H15" s="1">
-        <v>3.0366</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="I15" s="1">
-        <v>4.8520000000000003</v>
-      </c>
-      <c r="J15" s="1">
-        <v>7.7354000000000003</v>
-      </c>
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="J15" s="8"/>
       <c r="K15" s="1">
-        <v>8.2760999999999996</v>
-      </c>
-      <c r="L15" s="9"/>
+        <v>3.2559999999999998</v>
+      </c>
+      <c r="L15" s="1">
+        <v>1.5880000000000001</v>
+      </c>
       <c r="M15" s="1">
-        <v>3.2509999999999999</v>
+        <v>0.93</v>
       </c>
       <c r="N15" s="1">
-        <v>4.3079999999999998</v>
-      </c>
-      <c r="O15" s="1">
-        <v>6.681</v>
-      </c>
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="O15" s="8"/>
       <c r="P15" s="1">
-        <v>6.6829999999999998</v>
-      </c>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="1">
         <v>2.6019999999999999</v>
       </c>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
       <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
-        <f t="shared" ref="A16:F16" si="0">AVERAGE(A6:A15)</f>
-        <v>1.79619</v>
+        <f t="shared" ref="A16:D16" si="0">AVERAGE(A6:A15)</f>
+        <v>1.5499500000000002</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>0.98401139999999998</v>
+        <v>0.79174560000000005</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>0.62285650000000004</v>
+        <v>0.45439160000000001</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>0.66892819999999997</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.61754870000000017</v>
+        <v>0.45939300000000005</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="0"/>
-        <v>0.66545160000000003</v>
+        <f t="shared" ref="F16:I16" si="1">AVERAGE(F6:F15)</f>
+        <v>2.3837999999999999</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>1.2170000000000001</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" ref="H16:K16" si="1">AVERAGE(H6:H15)</f>
-        <v>3.1086</v>
+        <f t="shared" si="1"/>
+        <v>0.71250000000000013</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="1"/>
-        <v>4.9429629999999989</v>
-      </c>
-      <c r="J16" s="2">
-        <f t="shared" si="1"/>
-        <v>7.6752519999999986</v>
-      </c>
+        <v>0.73369999999999991</v>
+      </c>
+      <c r="J16" s="2"/>
       <c r="K16" s="2">
-        <f t="shared" si="1"/>
-        <v>8.192029999999999</v>
-      </c>
-      <c r="L16" s="2"/>
+        <f t="shared" ref="K16:N16" si="2">AVERAGE(K6:K15)</f>
+        <v>3.1560999999999995</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5948</v>
+      </c>
       <c r="M16" s="2">
-        <f t="shared" ref="M16:P16" si="2">AVERAGE(M6:M15)</f>
-        <v>3.3241999999999989</v>
+        <f t="shared" si="2"/>
+        <v>0.95479999999999998</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>4.2553000000000001</v>
-      </c>
-      <c r="O16" s="2">
-        <f t="shared" si="2"/>
-        <v>6.5561000000000007</v>
-      </c>
+        <v>0.96449999999999991</v>
+      </c>
+      <c r="O16" s="2"/>
       <c r="P16" s="2">
-        <f t="shared" si="2"/>
-        <v>6.6692000000000009</v>
+        <f t="shared" ref="P16" si="3">AVERAGE(P6:P15)</f>
+        <v>2.6150000000000002</v>
       </c>
       <c r="Q16" s="2"/>
-      <c r="R16" s="2">
-        <f t="shared" ref="R16" si="3">AVERAGE(R6:R15)</f>
-        <v>2.6150000000000002</v>
-      </c>
+      <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="6">
         <f>$A16/B16</f>
-        <v>1.825375193823974</v>
+        <v>1.9576363922957072</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" ref="C17:F17" si="4">$A16/C16</f>
-        <v>2.8837942607968285</v>
+        <f t="shared" ref="C17:D17" si="4">$A16/C16</f>
+        <v>3.4110445703661778</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="4"/>
-        <v>2.6851760771933373</v>
-      </c>
-      <c r="E17" s="6">
-        <f t="shared" si="4"/>
-        <v>2.9085803273490809</v>
-      </c>
-      <c r="F17" s="6">
-        <f t="shared" si="4"/>
-        <v>2.6992045702497371</v>
-      </c>
-      <c r="H17" s="5"/>
+        <v>3.3739086141930765</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="6">
+        <f>$F16/G16</f>
+        <v>1.9587510271158586</v>
+      </c>
+      <c r="H17" s="6">
+        <f t="shared" ref="H17:I17" si="5">$F16/H16</f>
+        <v>3.3456842105263149</v>
+      </c>
       <c r="I17" s="6">
-        <f>$H16/I16</f>
-        <v>0.62889404593965215</v>
-      </c>
-      <c r="J17" s="6">
-        <f t="shared" ref="J17:K17" si="5">$H16/J16</f>
-        <v>0.40501601771511875</v>
-      </c>
-      <c r="K17" s="6">
         <f t="shared" si="5"/>
-        <v>0.37946638379009845</v>
-      </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="5"/>
+        <v>3.2490118577075102</v>
+      </c>
+      <c r="J17" s="6"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="6">
+        <f>$F16/L16</f>
+        <v>1.4947328818660646</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" ref="M17:N17" si="6">$F16/M16</f>
+        <v>2.4966485127775448</v>
+      </c>
       <c r="N17" s="6">
-        <f>$H16/N16</f>
-        <v>0.73052428735929309</v>
-      </c>
-      <c r="O17" s="6">
-        <f t="shared" ref="O17:P17" si="6">$H16/O16</f>
-        <v>0.47415384146062439</v>
-      </c>
-      <c r="P17" s="6">
         <f t="shared" si="6"/>
-        <v>0.46611287710669941</v>
-      </c>
+        <v>2.4715396578538105</v>
+      </c>
+      <c r="O17" s="6"/>
+      <c r="P17" s="5"/>
       <c r="Q17" s="6"/>
-      <c r="R17" s="5"/>
+      <c r="R17" s="6"/>
       <c r="S17" s="6"/>
-      <c r="T17" s="6"/>
-      <c r="U17" s="6"/>
     </row>
-    <row r="18" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>16</v>
+    <row r="18" spans="1:19" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="C20" s="16" t="s">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="C20" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="16"/>
-      <c r="F20" s="16" t="s">
+      <c r="D20" s="18"/>
+      <c r="F20" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
+      <c r="H21" s="12" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="2">
         <f>$A$16</f>
-        <v>1.79619</v>
+        <v>1.5499500000000002</v>
       </c>
       <c r="C22" s="2">
-        <f>$H$16</f>
-        <v>3.1086</v>
+        <f>$F$16</f>
+        <v>2.3837999999999999</v>
       </c>
       <c r="D22" s="2">
-        <f>$M$16</f>
-        <v>3.3241999999999989</v>
+        <f>$K$16</f>
+        <v>3.1560999999999995</v>
       </c>
       <c r="E22" s="2">
-        <f>$R$16</f>
+        <f>$P$16</f>
         <v>2.6150000000000002</v>
       </c>
       <c r="F22">
@@ -1995,85 +2235,85 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23" s="2">
         <f>$B$16</f>
-        <v>0.98401139999999998</v>
+        <v>0.79174560000000005</v>
       </c>
       <c r="C23" s="2">
-        <f>$I$16</f>
-        <v>4.9429629999999989</v>
+        <f>$G$16</f>
+        <v>1.2170000000000001</v>
       </c>
       <c r="D23" s="2">
-        <f>$N$16</f>
-        <v>4.2553000000000001</v>
+        <f>$L$16</f>
+        <v>1.5948</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="B24" s="2">
-        <f>$E$16</f>
-        <v>0.61754870000000017</v>
+        <f>$C$16</f>
+        <v>0.45439160000000001</v>
       </c>
       <c r="C24" s="2">
-        <f>$J$16</f>
-        <v>7.6752519999999986</v>
+        <f>$H$16</f>
+        <v>0.71250000000000013</v>
       </c>
       <c r="D24" s="2">
-        <f>$O$16</f>
-        <v>6.5561000000000007</v>
+        <f>$M$16</f>
+        <v>0.95479999999999998</v>
       </c>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
       <c r="B25" s="2">
-        <f>$F$16</f>
-        <v>0.66545160000000003</v>
+        <f>$D$16</f>
+        <v>0.45939300000000005</v>
       </c>
       <c r="C25" s="2">
-        <f>$K$16</f>
-        <v>8.192029999999999</v>
+        <f>$I$16</f>
+        <v>0.73369999999999991</v>
       </c>
       <c r="D25" s="2">
-        <f>$P$16</f>
-        <v>6.6692000000000009</v>
+        <f>$N$16</f>
+        <v>0.96449999999999991</v>
       </c>
       <c r="E25" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="C20:D20"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="R3:U3"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:U4"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="B4:D4"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="K2:N2"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="landscape" copies="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="B16:D16 I16" formulaRange="1"/>
+    <ignoredError sqref="B16 G16" formulaRange="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor optimization in Kotlin
</commit_message>
<xml_diff>
--- a/doc/Results.xlsx
+++ b/doc/Results.xlsx
@@ -272,6 +272,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -280,12 +286,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,11 +671,11 @@
         </c:hiLowLines>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="233643392"/>
-        <c:axId val="233666048"/>
+        <c:axId val="208149504"/>
+        <c:axId val="208176256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="233643392"/>
+        <c:axId val="208149504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,7 +710,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="233666048"/>
+        <c:crossAx val="208176256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -718,7 +718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="233666048"/>
+        <c:axId val="208176256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3.5"/>
@@ -774,7 +774,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="233643392"/>
+        <c:crossAx val="208149504"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -967,11 +967,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="37035008"/>
-        <c:axId val="37161216"/>
+        <c:axId val="208077184"/>
+        <c:axId val="208078720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="37035008"/>
+        <c:axId val="208077184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -980,7 +980,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37161216"/>
+        <c:crossAx val="208078720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -988,7 +988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37161216"/>
+        <c:axId val="208078720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1005,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="37035008"/>
+        <c:crossAx val="208077184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O56" sqref="O56"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1519,97 +1519,97 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="F2" s="18" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="F2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="9"/>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
       <c r="O2" s="9"/>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="F3" s="17" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="F3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
       <c r="O3" s="10"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
     </row>
     <row r="4" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="F4" s="15" t="s">
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="F4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="11"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -1619,7 +1619,7 @@
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="3">
         <v>2</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="13"/>
-      <c r="K5" s="16"/>
+      <c r="K5" s="18"/>
       <c r="L5" s="3">
         <v>2</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>5</v>
       </c>
       <c r="O5" s="13"/>
-      <c r="P5" s="16"/>
+      <c r="P5" s="18"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3"/>
@@ -2178,15 +2178,15 @@
       <c r="D18" s="6"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="F20" s="18" t="s">
+      <c r="D20" s="15"/>
+      <c r="F20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B21" s="7" t="s">
@@ -2232,7 +2232,7 @@
         <v>1.87</v>
       </c>
       <c r="H22">
-        <v>9.1999999999999993</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -2291,12 +2291,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B3:D3"/>
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="P3:S3"/>
     <mergeCell ref="P4:P5"/>
@@ -2309,6 +2303,12 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:N4"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="256" orientation="landscape" copies="0" r:id="rId1"/>

</xml_diff>